<commit_message>
Pronto para iniciar as práticas no Galileo
Proposta de curso concluída. Teoria pedagógica explicada e Scrum também
</commit_message>
<xml_diff>
--- a/artigos, livros referencia/Scrum X edu.xlsx
+++ b/artigos, livros referencia/Scrum X edu.xlsx
@@ -944,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>